<commit_message>
Weapon editor and selector updated
</commit_message>
<xml_diff>
--- a/Data/Advantages.xlsx
+++ b/Data/Advantages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\source\repos\DaemonMitica\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2524280-C263-4F69-A82E-1B0E9639C65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2E7FD8-74A0-41FA-B517-8703B90347C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="2100" windowWidth="21915" windowHeight="11940" xr2:uid="{EC9EDA72-4F59-4457-81A4-AF652A3AB1C0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC9EDA72-4F59-4457-81A4-AF652A3AB1C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="153">
   <si>
     <t>Description</t>
   </si>
@@ -507,6 +507,40 @@
   </si>
   <si>
     <t>O senhor ou Daimyo é considerado indigno de confiança, é avarento, ou talvez trate mal os seus servos, mas independente dos motivos ele é detestado por muitos membros do regime de Shogunato ou dentro de um clã de samurais. O fato de você estar servindo a este senhor lhe traz muitos problemas, pois as pessoas tendem a te tratar mal. Ainda assim você segue seu senhor.</t>
+  </si>
+  <si>
+    <t>Alvo Elusivo (1)</t>
+  </si>
+  <si>
+    <t>Alvo Elusivo (2)</t>
+  </si>
+  <si>
+    <t>O personagem, quando em combate corpo-a-corpo, consegue usar seus oponentes comocobertura, bloqueando e atrapalhando os ataques de inimigos. Sempre que estiver enfrentando mais de um oponente ao mesmo tempo, o personagem é capaz de se posicionar de modo a atrapalhar os ataques dos outros inimigos.
+Cada um dos oponentes recebe uma penalidade de 30% em ataque. Não pode ser usado contra armas de
+longa distância.</t>
+  </si>
+  <si>
+    <t>O personagem, quando em combate corpo-a-corpo, consegue usar seus oponentes comocobertura, bloqueando e atrapalhando os ataques de inimigos. Sempre que estiver enfrentando mais de um oponente ao mesmo tempo, o personagem é capaz de se posicionar de modo a atrapalhar os ataques dos outros inimigos.
+Cada um dos oponentes recebe uma penalidade de 20% em ataque. Não pode ser usado contra armas de
+longa distância.</t>
+  </si>
+  <si>
+    <t>Amor verdadeiro</t>
+  </si>
+  <si>
+    <t>Você ama alguém do fundo do seu coração, e não importa o que ou quem tente interferir neste relacionamento, nada abalará o amor mútuo entre vocês sentem um pelo outro. Independente da situação, você vai ter forças para defender seu amor.
+Em toda a situação que a pessoa que você ama estiver em apuros, o personagem recebe um bônus especial de +10% em todos os seus Testes de Atributos Físicos e Perícias que forem realizados na tentativa de ajudá-la. também torna todos os seus Testes de WILL Fáceis contra Sedução.</t>
+  </si>
+  <si>
+    <t>Aparência Inofensiva</t>
+  </si>
+  <si>
+    <t>Você não aparenta ser perigoso. Na verdade, os oponentes menosprezam sua presença, ninguém acredita que você seja capaz de realizar algum grande feito e dificilmente o tomarão como uma ameaça (a não ser aqueles que já conhecem o Personagem há tempo suficiente para saber se isso é verdade ou não). Considere que o personagem automaticamente vence a Iniciativa quando um combate começar.
+Porém, depois de enfrentar um adversário uma vez, ele poderá já estar ciente do seu potencial e
+não lhe permitirá nenhuma vantagem (então a Iniciativa deve ser testada normalmente).</t>
+  </si>
+  <si>
+    <t>Ataque</t>
   </si>
 </sst>
 </file>
@@ -590,8 +624,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB99BE2A-770B-4854-B7AC-2BC0076CE99A}" name="Table1" displayName="Table1" ref="A1:D71" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D71" xr:uid="{FB99BE2A-770B-4854-B7AC-2BC0076CE99A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB99BE2A-770B-4854-B7AC-2BC0076CE99A}" name="Table1" displayName="Table1" ref="A1:D76" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D76" xr:uid="{FB99BE2A-770B-4854-B7AC-2BC0076CE99A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9A989A95-4D0C-42FD-A58C-5B7EAF5CB39A}" name="Name" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{602CB169-BA77-4103-B754-03EC7B7C025F}" name="Cost" dataDxfId="2"/>
@@ -919,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206669F2-BFFD-4434-B009-480A1A95BDDD}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,6 +1761,55 @@
         <v>143</v>
       </c>
     </row>
+    <row r="72" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>